<commit_message>
Draft final interim report 2
</commit_message>
<xml_diff>
--- a/cost_benefit_TCedits.xlsx
+++ b/cost_benefit_TCedits.xlsx
@@ -2985,8 +2985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="BA4" sqref="BA4"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="BC11" sqref="BC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,78 +3549,78 @@
         <v>129415143.10091935</v>
       </c>
       <c r="AI5" s="2">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="AJ5" s="2">
         <v>10</v>
       </c>
       <c r="AK5" s="2">
         <f>AJ5*AI5</f>
-        <v>1750</v>
+        <v>1450</v>
       </c>
       <c r="AL5" s="2">
         <f>AK5*0.17</f>
-        <v>297.5</v>
+        <v>246.50000000000003</v>
       </c>
       <c r="AM5" s="2">
         <f t="shared" ref="AM5:AM17" si="10">AL5*V5+AK5*S5</f>
-        <v>1999725</v>
+        <v>1656915</v>
       </c>
       <c r="AN5" s="2">
         <f t="shared" ref="AN5:AN17" si="11">(R5-AK5)</f>
-        <v>127151</v>
+        <v>127451</v>
       </c>
       <c r="AO5" s="2">
         <f t="shared" si="6"/>
-        <v>14529544.77</v>
+        <v>14563825.77</v>
       </c>
       <c r="AP5" s="2">
         <f t="shared" si="6"/>
-        <v>14106354.145631067</v>
+        <v>14139636.669902913</v>
       </c>
       <c r="AQ5" s="2">
         <f t="shared" si="6"/>
-        <v>13695489.461777736</v>
+        <v>13727802.59213875</v>
       </c>
       <c r="AR5" s="2">
         <f t="shared" si="6"/>
-        <v>13296591.710463822</v>
+        <v>13327963.681688108</v>
       </c>
       <c r="AS5" s="2">
         <f t="shared" si="6"/>
-        <v>12909312.340256138</v>
+        <v>12939770.564745735</v>
       </c>
       <c r="AT5" s="2">
         <f t="shared" si="6"/>
-        <v>12533312.951704988</v>
+        <v>12562884.043442462</v>
       </c>
       <c r="AU5" s="2">
         <f t="shared" si="6"/>
-        <v>12168265.001655329</v>
+        <v>12196974.799458701</v>
       </c>
       <c r="AV5" s="2">
         <f t="shared" si="6"/>
-        <v>11813849.51617022</v>
+        <v>11841723.106270583</v>
       </c>
       <c r="AW5" s="2">
         <f t="shared" si="6"/>
-        <v>11469756.81181575</v>
+        <v>11496818.549777266</v>
       </c>
       <c r="AX5" s="2">
         <f t="shared" si="6"/>
-        <v>11135686.225063834</v>
+        <v>11161959.757065305</v>
       </c>
       <c r="AY5" s="2">
         <f>SUM(AO5:AX5)</f>
-        <v>127658162.93453889</v>
+        <v>127959359.53448983</v>
       </c>
       <c r="AZ5" s="2">
         <f t="shared" ref="AZ5:AZ17" si="12">AY5-Q5</f>
-        <v>126058162.93453889</v>
+        <v>126359359.53448983</v>
       </c>
       <c r="BA5" s="3">
         <f>AY5/Q5</f>
-        <v>79.786351834086801</v>
+        <v>79.974599709056136</v>
       </c>
       <c r="BB5" s="2"/>
       <c r="BC5" s="3"/>
@@ -3747,78 +3747,78 @@
         <v>129415143.10091935</v>
       </c>
       <c r="AI6" s="2">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="AJ6" s="2">
         <v>10</v>
       </c>
       <c r="AK6" s="2">
         <f t="shared" ref="AK6:AK8" si="15">AJ6*AI6</f>
-        <v>1750</v>
+        <v>1450</v>
       </c>
       <c r="AL6" s="2">
         <f t="shared" ref="AL6:AL8" si="16">AK6*0.17</f>
-        <v>297.5</v>
+        <v>246.50000000000003</v>
       </c>
       <c r="AM6" s="2">
         <f t="shared" si="10"/>
-        <v>1999725</v>
+        <v>1656915</v>
       </c>
       <c r="AN6" s="2">
         <f t="shared" si="11"/>
-        <v>127151</v>
+        <v>127451</v>
       </c>
       <c r="AO6" s="2">
         <f t="shared" si="6"/>
-        <v>14529544.77</v>
+        <v>14563825.77</v>
       </c>
       <c r="AP6" s="2">
         <f t="shared" si="6"/>
-        <v>14106354.145631067</v>
+        <v>14139636.669902913</v>
       </c>
       <c r="AQ6" s="2">
         <f t="shared" si="6"/>
-        <v>13695489.461777736</v>
+        <v>13727802.59213875</v>
       </c>
       <c r="AR6" s="2">
         <f t="shared" si="6"/>
-        <v>13296591.710463822</v>
+        <v>13327963.681688108</v>
       </c>
       <c r="AS6" s="2">
         <f t="shared" si="6"/>
-        <v>12909312.340256138</v>
+        <v>12939770.564745735</v>
       </c>
       <c r="AT6" s="2">
         <f t="shared" si="6"/>
-        <v>12533312.951704988</v>
+        <v>12562884.043442462</v>
       </c>
       <c r="AU6" s="2">
         <f t="shared" si="6"/>
-        <v>12168265.001655329</v>
+        <v>12196974.799458701</v>
       </c>
       <c r="AV6" s="2">
         <f t="shared" si="6"/>
-        <v>11813849.51617022</v>
+        <v>11841723.106270583</v>
       </c>
       <c r="AW6" s="2">
         <f t="shared" si="6"/>
-        <v>11469756.81181575</v>
+        <v>11496818.549777266</v>
       </c>
       <c r="AX6" s="2">
         <f t="shared" si="6"/>
-        <v>11135686.225063834</v>
+        <v>11161959.757065305</v>
       </c>
       <c r="AY6" s="2">
         <f t="shared" ref="AY6:AY17" si="17">SUM(AO6:AX6)</f>
-        <v>127658162.93453889</v>
+        <v>127959359.53448983</v>
       </c>
       <c r="AZ6" s="2">
         <f t="shared" si="12"/>
-        <v>123658162.93453889</v>
+        <v>123959359.53448983</v>
       </c>
       <c r="BA6" s="3">
         <f t="shared" ref="BA6:BA17" si="18">AY6/Q6</f>
-        <v>31.91454073363472</v>
+        <v>31.989839883622455</v>
       </c>
       <c r="BB6" s="2"/>
       <c r="BC6" s="3"/>
@@ -4667,7 +4667,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="2">
-        <v>2200</v>
+        <v>130</v>
       </c>
       <c r="S11">
         <v>852</v>
@@ -4678,58 +4678,58 @@
       </c>
       <c r="U11" s="2">
         <f>R11*T11</f>
-        <v>374</v>
+        <v>22.1</v>
       </c>
       <c r="V11" s="2">
         <v>1710</v>
       </c>
       <c r="W11" s="2">
         <f t="shared" si="8"/>
-        <v>2513940</v>
+        <v>148551</v>
       </c>
       <c r="X11" s="2">
         <f t="shared" si="5"/>
-        <v>251394</v>
+        <v>14855.1</v>
       </c>
       <c r="Y11" s="2">
         <f t="shared" si="5"/>
-        <v>244071.84466019418</v>
+        <v>14422.42718446602</v>
       </c>
       <c r="Z11" s="2">
         <f t="shared" si="5"/>
-        <v>236962.95598077105</v>
+        <v>14002.356489772834</v>
       </c>
       <c r="AA11" s="2">
         <f t="shared" si="5"/>
-        <v>230061.12231142822</v>
+        <v>13594.520863857122</v>
       </c>
       <c r="AB11" s="2">
         <f t="shared" si="5"/>
-        <v>223360.31292371673</v>
+        <v>13198.563945492351</v>
       </c>
       <c r="AC11" s="2">
         <f t="shared" si="5"/>
-        <v>216854.67274147255</v>
+        <v>12814.139752905197</v>
       </c>
       <c r="AD11" s="2">
         <f t="shared" si="5"/>
-        <v>210538.51722473063</v>
+        <v>12440.912381461356</v>
       </c>
       <c r="AE11" s="2">
         <f t="shared" si="5"/>
-        <v>204406.32740265108</v>
+        <v>12078.555710156656</v>
       </c>
       <c r="AF11" s="2">
         <f t="shared" si="5"/>
-        <v>198452.74505111756</v>
+        <v>11726.753116656946</v>
       </c>
       <c r="AG11" s="2">
         <f t="shared" si="5"/>
-        <v>192672.56801079377</v>
+        <v>11385.197200637813</v>
       </c>
       <c r="AH11" s="2">
         <f t="shared" si="9"/>
-        <v>2208775.066306876</v>
+        <v>130518.52664540627</v>
       </c>
       <c r="AI11" s="2">
         <v>13</v>
@@ -4751,55 +4751,55 @@
       </c>
       <c r="AN11" s="2">
         <f t="shared" si="11"/>
-        <v>2070</v>
+        <v>0</v>
       </c>
       <c r="AO11" s="2">
         <f t="shared" si="6"/>
-        <v>236538.9</v>
+        <v>0</v>
       </c>
       <c r="AP11" s="2">
         <f t="shared" si="6"/>
-        <v>229649.41747572814</v>
+        <v>0</v>
       </c>
       <c r="AQ11" s="2">
         <f t="shared" si="6"/>
-        <v>222960.5994909982</v>
+        <v>0</v>
       </c>
       <c r="AR11" s="2">
         <f t="shared" si="6"/>
-        <v>216466.60144757107</v>
+        <v>0</v>
       </c>
       <c r="AS11" s="2">
         <f t="shared" si="6"/>
-        <v>210161.74897822435</v>
+        <v>0</v>
       </c>
       <c r="AT11" s="2">
         <f t="shared" si="6"/>
-        <v>204040.53298856734</v>
+        <v>0</v>
       </c>
       <c r="AU11" s="2">
         <f t="shared" si="6"/>
-        <v>198097.60484326928</v>
+        <v>0</v>
       </c>
       <c r="AV11" s="2">
         <f t="shared" si="6"/>
-        <v>192327.77169249443</v>
+        <v>0</v>
       </c>
       <c r="AW11" s="2">
         <f t="shared" si="6"/>
-        <v>186725.99193446062</v>
+        <v>0</v>
       </c>
       <c r="AX11" s="2">
         <f t="shared" si="6"/>
-        <v>181287.37081015593</v>
+        <v>0</v>
       </c>
       <c r="AY11" s="2">
         <f t="shared" si="17"/>
-        <v>2078256.5396614694</v>
+        <v>0</v>
       </c>
       <c r="AZ11" s="2">
         <f>AY11-Q11</f>
-        <v>2078256.5396614694</v>
+        <v>0</v>
       </c>
       <c r="BA11" s="3" t="e">
         <f t="shared" si="18"/>
@@ -4930,78 +4930,78 @@
         <v>2208775.066306876</v>
       </c>
       <c r="AI12" s="2">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="AJ12" s="2">
         <v>10</v>
       </c>
       <c r="AK12" s="2">
         <f>AJ12*AI12</f>
-        <v>1750</v>
+        <v>1450</v>
       </c>
       <c r="AL12" s="2">
         <f>AK12*0.17</f>
-        <v>297.5</v>
+        <v>246.50000000000003</v>
       </c>
       <c r="AM12" s="2">
         <f t="shared" si="10"/>
-        <v>1999725</v>
+        <v>1656915</v>
       </c>
       <c r="AN12" s="2">
         <f t="shared" si="11"/>
-        <v>450</v>
+        <v>750</v>
       </c>
       <c r="AO12" s="2">
         <f t="shared" si="6"/>
-        <v>51421.5</v>
+        <v>85702.5</v>
       </c>
       <c r="AP12" s="2">
         <f t="shared" si="6"/>
-        <v>49923.786407766987</v>
+        <v>83206.310679611648</v>
       </c>
       <c r="AQ12" s="2">
         <f t="shared" si="6"/>
-        <v>48469.695541521352</v>
+        <v>80782.82590253558</v>
       </c>
       <c r="AR12" s="2">
         <f t="shared" si="6"/>
-        <v>47057.956836428493</v>
+        <v>78429.928060714155</v>
       </c>
       <c r="AS12" s="2">
         <f t="shared" si="6"/>
-        <v>45687.336734396602</v>
+        <v>76145.561223994329</v>
       </c>
       <c r="AT12" s="2">
         <f t="shared" si="6"/>
-        <v>44356.637606210294</v>
+        <v>73927.729343683823</v>
       </c>
       <c r="AU12" s="2">
         <f t="shared" si="6"/>
-        <v>43064.696705058537</v>
+        <v>71774.4945084309</v>
       </c>
       <c r="AV12" s="2">
         <f t="shared" si="6"/>
-        <v>41810.385150542264</v>
+        <v>69683.975250903779</v>
       </c>
       <c r="AW12" s="2">
         <f t="shared" si="6"/>
-        <v>40592.606942274047</v>
+        <v>67654.344903790072</v>
       </c>
       <c r="AX12" s="2">
         <f t="shared" si="6"/>
-        <v>39410.298002207812</v>
+        <v>65683.830003679686</v>
       </c>
       <c r="AY12" s="2">
         <f t="shared" si="17"/>
-        <v>451794.89992640639</v>
+        <v>752991.499877344</v>
       </c>
       <c r="AZ12" s="2">
         <f t="shared" si="12"/>
-        <v>-1148205.1000735937</v>
+        <v>-847008.500122656</v>
       </c>
       <c r="BA12" s="3">
         <f t="shared" si="18"/>
-        <v>0.282371812454004</v>
+        <v>0.47061968742333998</v>
       </c>
       <c r="BB12" s="2"/>
       <c r="BC12" s="3"/>
@@ -5128,78 +5128,78 @@
         <v>2208775.066306876</v>
       </c>
       <c r="AI13" s="2">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="AJ13" s="2">
         <v>10</v>
       </c>
       <c r="AK13" s="2">
         <f t="shared" ref="AK13:AK15" si="21">AJ13*AI13</f>
-        <v>1750</v>
+        <v>1450</v>
       </c>
       <c r="AL13" s="2">
         <f t="shared" ref="AL13:AL15" si="22">AK13*0.17</f>
-        <v>297.5</v>
+        <v>246.50000000000003</v>
       </c>
       <c r="AM13" s="2">
         <f t="shared" si="10"/>
-        <v>1999725</v>
+        <v>1656915</v>
       </c>
       <c r="AN13" s="2">
         <f t="shared" si="11"/>
-        <v>450</v>
+        <v>750</v>
       </c>
       <c r="AO13" s="2">
         <f t="shared" si="6"/>
-        <v>51421.5</v>
+        <v>85702.5</v>
       </c>
       <c r="AP13" s="2">
         <f t="shared" si="6"/>
-        <v>49923.786407766987</v>
+        <v>83206.310679611648</v>
       </c>
       <c r="AQ13" s="2">
         <f t="shared" si="6"/>
-        <v>48469.695541521352</v>
+        <v>80782.82590253558</v>
       </c>
       <c r="AR13" s="2">
         <f t="shared" si="6"/>
-        <v>47057.956836428493</v>
+        <v>78429.928060714155</v>
       </c>
       <c r="AS13" s="2">
         <f t="shared" si="6"/>
-        <v>45687.336734396602</v>
+        <v>76145.561223994329</v>
       </c>
       <c r="AT13" s="2">
         <f t="shared" si="6"/>
-        <v>44356.637606210294</v>
+        <v>73927.729343683823</v>
       </c>
       <c r="AU13" s="2">
         <f t="shared" si="6"/>
-        <v>43064.696705058537</v>
+        <v>71774.4945084309</v>
       </c>
       <c r="AV13" s="2">
         <f t="shared" si="6"/>
-        <v>41810.385150542264</v>
+        <v>69683.975250903779</v>
       </c>
       <c r="AW13" s="2">
         <f t="shared" si="6"/>
-        <v>40592.606942274047</v>
+        <v>67654.344903790072</v>
       </c>
       <c r="AX13" s="2">
         <f t="shared" si="6"/>
-        <v>39410.298002207812</v>
+        <v>65683.830003679686</v>
       </c>
       <c r="AY13" s="2">
         <f t="shared" si="17"/>
-        <v>451794.89992640639</v>
+        <v>752991.499877344</v>
       </c>
       <c r="AZ13" s="2">
         <f t="shared" si="12"/>
-        <v>-3548205.1000735937</v>
+        <v>-3247008.5001226561</v>
       </c>
       <c r="BA13" s="3">
         <f t="shared" si="18"/>
-        <v>0.11294872498160159</v>
+        <v>0.18824787496933601</v>
       </c>
       <c r="BB13" s="2"/>
       <c r="BC13" s="3"/>

</xml_diff>